<commit_message>
Bugfix for relative density categories
</commit_message>
<xml_diff>
--- a/notebooks/Data/WFS1-2_cone_props.xlsx
+++ b/notebooks/Data/WFS1-2_cone_props.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/SourceTree.tmp/ProFound/groundhog/notebooks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32DCC22-A096-8241-9CA8-5D3A8A694A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F6B6F-C84F-DA4D-A434-3EAA110F3B4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="0" windowWidth="24760" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>